<commit_message>
Added new setup excel.
Added new setup excel.
</commit_message>
<xml_diff>
--- a/hans_vcsel_mask/layer_definition_v2.xlsx
+++ b/hans_vcsel_mask/layer_definition_v2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kaimre\Documents\GitHub\SELMA\hans_vcsel_mask\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4C9A4A0-F81F-4231-95D9-BC1DFE0E4EFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C212DFD5-3AEB-4309-A3DA-7C8CDC83331F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="39">
   <si>
     <t>data_parity</t>
   </si>
@@ -93,9 +93,6 @@
     <t>NO_LABEL</t>
   </si>
   <si>
-    <t>5. BOTTOM CONTACT  (DC)</t>
-  </si>
-  <si>
     <t>bcb</t>
   </si>
   <si>
@@ -108,28 +105,43 @@
     <t>4. BOTTOM MESA (DD)</t>
   </si>
   <si>
-    <t>6. CONTACT ETCH  (DD)</t>
-  </si>
-  <si>
-    <t>8. BCB ETCH CONT (DC)</t>
-  </si>
-  <si>
-    <t>9. SiNx ON BCB (DC)</t>
-  </si>
-  <si>
     <t>bondpads</t>
   </si>
   <si>
-    <t>10. PADS  (DC)</t>
-  </si>
-  <si>
-    <t>11. BONDPADS (DC)</t>
-  </si>
-  <si>
     <t>bottom_mesa</t>
   </si>
   <si>
     <t>7. BCB ETCH (DD)</t>
+  </si>
+  <si>
+    <t>8A. BCB ETCH CONT (DC)</t>
+  </si>
+  <si>
+    <t>bcb_etch_mesa_15-21</t>
+  </si>
+  <si>
+    <t>bcb_etch_mesa_17-23</t>
+  </si>
+  <si>
+    <t>8D. SiNx ON BCB (DC)</t>
+  </si>
+  <si>
+    <t>9. PADS  (DC)</t>
+  </si>
+  <si>
+    <t>10. BONDPADS (DC)</t>
+  </si>
+  <si>
+    <t>5. BOTTOM CONTACT(DC)</t>
+  </si>
+  <si>
+    <t>6. CONTACT ETCH(DD)</t>
+  </si>
+  <si>
+    <t>8B. BCB MESA 15-21(DC)</t>
+  </si>
+  <si>
+    <t>8C. BCB MESA 17-23(DC)</t>
   </si>
 </sst>
 </file>
@@ -447,20 +459,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="23.28515625" customWidth="1"/>
     <col min="2" max="2" width="22.5703125" customWidth="1"/>
     <col min="3" max="3" width="20.5703125" customWidth="1"/>
     <col min="4" max="4" width="25.28515625" customWidth="1"/>
     <col min="5" max="5" width="25.7109375" customWidth="1"/>
-    <col min="6" max="6" width="30.42578125" customWidth="1"/>
+    <col min="6" max="6" width="37.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -545,7 +557,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -560,7 +572,7 @@
         <v>0</v>
       </c>
       <c r="F5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -580,7 +592,7 @@
         <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -600,12 +612,12 @@
         <v>0</v>
       </c>
       <c r="F7" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -620,12 +632,12 @@
         <v>0</v>
       </c>
       <c r="F8" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -640,12 +652,12 @@
         <v>0</v>
       </c>
       <c r="F9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -654,18 +666,18 @@
         <v>17</v>
       </c>
       <c r="D10">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E10">
         <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -674,18 +686,18 @@
         <v>17</v>
       </c>
       <c r="D11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E11">
         <v>0</v>
       </c>
       <c r="F11" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -705,53 +717,53 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B13">
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" t="s">
-        <v>9</v>
+        <v>17</v>
+      </c>
+      <c r="D13">
+        <v>6</v>
       </c>
       <c r="E13">
         <v>0</v>
       </c>
       <c r="F13" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="B14">
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" t="s">
-        <v>9</v>
+        <v>17</v>
+      </c>
+      <c r="D14">
+        <v>8</v>
       </c>
       <c r="E14">
         <v>0</v>
       </c>
       <c r="F14" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B15">
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D15" t="s">
         <v>9</v>
@@ -763,7 +775,48 @@
         <v>21</v>
       </c>
     </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17">
+        <v>16</v>
+      </c>
+      <c r="C17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Hot Optics mask pre-final.
</commit_message>
<xml_diff>
--- a/hans_vcsel_mask/layer_definition_v2.xlsx
+++ b/hans_vcsel_mask/layer_definition_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kaimre\Documents\GitHub\SELMA\hans_vcsel_mask\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C212DFD5-3AEB-4309-A3DA-7C8CDC83331F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02B3B57C-AA0A-436A-8E85-86AC4BA47793}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="50">
   <si>
     <t>data_parity</t>
   </si>
@@ -142,6 +142,39 @@
   </si>
   <si>
     <t>8C. BCB MESA 17-23(DC)</t>
+  </si>
+  <si>
+    <t>order_position</t>
+  </si>
+  <si>
+    <t>1.10</t>
+  </si>
+  <si>
+    <t>2.5</t>
+  </si>
+  <si>
+    <t>1.4</t>
+  </si>
+  <si>
+    <t>2.6</t>
+  </si>
+  <si>
+    <t>3.7</t>
+  </si>
+  <si>
+    <t>8.9</t>
+  </si>
+  <si>
+    <t>10.11</t>
+  </si>
+  <si>
+    <t>12.13</t>
+  </si>
+  <si>
+    <t>14.15</t>
+  </si>
+  <si>
+    <t>4.8</t>
   </si>
 </sst>
 </file>
@@ -459,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -473,9 +506,10 @@
     <col min="4" max="4" width="25.28515625" customWidth="1"/>
     <col min="5" max="5" width="25.7109375" customWidth="1"/>
     <col min="6" max="6" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -494,8 +528,11 @@
       <c r="F1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -514,8 +551,11 @@
       <c r="F2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -534,8 +574,11 @@
       <c r="F3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -554,8 +597,11 @@
       <c r="F4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -574,8 +620,11 @@
       <c r="F5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -594,8 +643,11 @@
       <c r="F6" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -614,8 +666,11 @@
       <c r="F7" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -634,8 +689,11 @@
       <c r="F8" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -654,8 +712,11 @@
       <c r="F9" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -674,8 +735,11 @@
       <c r="F10" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -694,8 +758,11 @@
       <c r="F11" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -714,8 +781,11 @@
       <c r="F12" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -734,8 +804,11 @@
       <c r="F13" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -754,8 +827,11 @@
       <c r="F14" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -774,8 +850,11 @@
       <c r="F15" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -794,8 +873,11 @@
       <c r="F16" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -813,6 +895,9 @@
       </c>
       <c r="F17" t="s">
         <v>21</v>
+      </c>
+      <c r="G17" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>